<commit_message>
fix import question and has Role
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/question_import_template.xlsx
+++ b/src/main/resources/templates/excel/question_import_template.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edu\BE_MONO\mono-services\src\main\resources\templates\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\code\backup\DoAn\BE_MONO\education\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543076A4-502D-48B6-9D69-D938C53E58E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="782" activeTab="1"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách câu hỏi" sheetId="1" r:id="rId1"/>
-    <sheet name="Danh sách nhóm câu hỏi" sheetId="2" r:id="rId2"/>
+    <sheet name="Danh sách nhóm câu hỏi" sheetId="3" r:id="rId2"/>
+    <sheet name="Mức độ câu hỏi" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,13 +27,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>sang nguyen</author>
     <author>admin</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E728D200-1F07-4C3F-9B44-A02E4D8E363B}">
       <text>
         <r>
           <rPr>
@@ -55,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1" shapeId="0">
+    <comment ref="A3" authorId="1" shapeId="0" xr:uid="{80D7E04B-B7DE-4C1C-8D92-108A2BDE541C}">
       <text>
         <r>
           <rPr>
@@ -83,8 +85,67 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>sang nguyen</author>
+    <author>admin</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sang nguyen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell = "C3")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="questionTypes", var="item", varIndex="i", lastCell="C3")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>${i+1}</t>
   </si>
@@ -98,12 +159,6 @@
     <t>${item.name}</t>
   </si>
   <si>
-    <t>Danh sách Nhóm câu hỏi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mã </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tên </t>
   </si>
   <si>
@@ -135,6 +190,15 @@
   </si>
   <si>
     <t>ĐA</t>
+  </si>
+  <si>
+    <t>Danh sách mức độ câu hỏi</t>
+  </si>
+  <si>
+    <t>Mã</t>
+  </si>
+  <si>
+    <t>Danh sách nhóm câu hỏi</t>
   </si>
   <si>
     <t>${item.subject.code}</t>
@@ -143,7 +207,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -244,11 +308,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -278,16 +386,37 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -603,7 +732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
@@ -623,49 +752,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="A1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -678,11 +807,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468C510C-68AD-454E-92EC-693DD2AAA91F}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,39 +824,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
-    <row r="2" spans="1:4" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
+      <c r="B2" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>17</v>
+      <c r="D3" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -737,4 +866,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>